<commit_message>
Add scripts for validation data feature
</commit_message>
<xml_diff>
--- a/ui-testsuite/src/main/resources/TestData/ATR_Imported_Anniversary_CheckFormatFields.xlsx
+++ b/ui-testsuite/src/main/resources/TestData/ATR_Imported_Anniversary_CheckFormatFields.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9018" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="349">
   <si>
     <t>IB TYPE</t>
   </si>
@@ -1532,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EP91" workbookViewId="0">
-      <selection activeCell="FA96" sqref="FA96"/>
+    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
+      <selection activeCell="DS10" sqref="DS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20174,22 +20174,22 @@
         <v>1.4</v>
       </c>
       <c r="CQ50" s="20">
-        <v>3644.3879452054798</v>
+        <v>-3644.3879452054798</v>
       </c>
       <c r="CR50" s="20">
-        <v>2603.1342465753428</v>
-      </c>
-      <c r="CS50" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT50" s="16">
-        <v>0</v>
+        <v>-12603.1342465753</v>
+      </c>
+      <c r="CS50" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="CT50" s="16" t="s">
+        <v>312</v>
       </c>
       <c r="CU50" s="20">
-        <v>3644.3879452054798</v>
+        <v>-3644.3879452054798</v>
       </c>
       <c r="CV50" s="20">
-        <v>2603.1342465753428</v>
+        <v>-2603.1342465753401</v>
       </c>
       <c r="CW50" s="24" t="s">
         <v>330</v>

</xml_diff>